<commit_message>
Update MasterCodebook_Final_June2022 ALL (Repaired) Back up Oct 19.xlsx
</commit_message>
<xml_diff>
--- a/1_Input_data/MasterCodebook_Final_June2022 ALL (Repaired) Back up Oct 19.xlsx
+++ b/1_Input_data/MasterCodebook_Final_June2022 ALL (Repaired) Back up Oct 19.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jdamen/Documents/GitHub/Zika_imputation/1_Input_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EE7660D7-8980-EB40-A929-27519C29F0B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67DC9895-EA9A-9D4B-A75B-5B2D54DB4483}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="36460" windowHeight="21840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,9 +26,9 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="Filter 1" guid="{3AF2D2F3-3B31-4BFE-9B21-6EF5937D96DE}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 3" guid="{9C9CF54D-CE09-4329-9468-764052FC28B8}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Filter 2" guid="{EB9D8945-92F8-48A6-B1A8-0874D0F705AD}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 3" guid="{9C9CF54D-CE09-4329-9468-764052FC28B8}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 1" guid="{3AF2D2F3-3B31-4BFE-9B21-6EF5937D96DE}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -48065,10 +48065,10 @@
   <dimension ref="A1:W282"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B228" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M241" sqref="M241"/>
+      <selection pane="bottomRight" activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1"/>

</xml_diff>